<commit_message>
Final testing on contract playbook
</commit_message>
<xml_diff>
--- a/all-aci-config.xlsx
+++ b/all-aci-config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="14"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="tenant-tn-vrf" sheetId="1" state="visible" r:id="rId2"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="215">
   <si>
     <t xml:space="preserve">tenant</t>
   </si>
@@ -582,27 +582,15 @@
     <t xml:space="preserve">protocol</t>
   </si>
   <si>
-    <t xml:space="preserve">fragsonly</t>
-  </si>
-  <si>
     <t xml:space="preserve">stateful</t>
   </si>
   <si>
-    <t xml:space="preserve">sourceportfrom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sourceportto</t>
-  </si>
-  <si>
     <t xml:space="preserve">destportfrom</t>
   </si>
   <si>
     <t xml:space="preserve">destportto</t>
   </si>
   <si>
-    <t xml:space="preserve">tcprules</t>
-  </si>
-  <si>
     <t xml:space="preserve">Permit-any</t>
   </si>
   <si>
@@ -685,9 +673,6 @@
   </si>
   <si>
     <t xml:space="preserve">cnttype</t>
-  </si>
-  <si>
-    <t xml:space="preserve">n/a</t>
   </si>
   <si>
     <t xml:space="preserve">provider</t>
@@ -798,10 +783,10 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D10 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.02"/>
@@ -923,10 +908,10 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D10 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.44"/>
@@ -1055,15 +1040,15 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="1" sqref="D10 E2"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.16"/>
@@ -1206,10 +1191,10 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="D10 B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.24"/>
@@ -1328,26 +1313,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="D10 B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="9.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="10.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="7.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="0" width="10.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="7.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="7.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1382,18 +1364,6 @@
         <v>184</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>185</v>
-      </c>
-      <c r="L1" s="0" t="s">
-        <v>186</v>
-      </c>
-      <c r="M1" s="0" t="s">
-        <v>187</v>
-      </c>
-      <c r="N1" s="0" t="s">
-        <v>188</v>
-      </c>
-      <c r="O1" s="0" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1402,45 +1372,33 @@
         <v>7</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="F2" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="C2" s="0" t="s">
-        <v>190</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>191</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>192</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>193</v>
-      </c>
       <c r="G2" s="0" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="H2" s="0" t="s">
         <v>44</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>44</v>
+        <v>189</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>193</v>
-      </c>
-      <c r="L2" s="0" t="s">
-        <v>193</v>
-      </c>
-      <c r="M2" s="0" t="s">
-        <v>193</v>
-      </c>
-      <c r="N2" s="0" t="s">
-        <v>193</v>
-      </c>
-      <c r="O2" s="0" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1449,45 +1407,33 @@
         <v>7</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="F3" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="G3" s="0" t="s">
         <v>193</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>197</v>
       </c>
       <c r="H3" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="I3" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>193</v>
+      <c r="I3" s="0" t="n">
+        <v>53</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>53</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>193</v>
-      </c>
-      <c r="L3" s="0" t="n">
-        <v>53</v>
-      </c>
-      <c r="M3" s="0" t="n">
-        <v>53</v>
-      </c>
-      <c r="N3" s="0" t="s">
-        <v>193</v>
-      </c>
-      <c r="O3" s="0" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1496,45 +1442,33 @@
         <v>7</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="D4" s="0" t="s">
         <v>194</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="E4" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="G4" s="0" t="s">
         <v>195</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>198</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>192</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>193</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>199</v>
       </c>
       <c r="H4" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="I4" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="J4" s="0" t="s">
-        <v>193</v>
+      <c r="I4" s="0" t="n">
+        <v>53</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>53</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>193</v>
-      </c>
-      <c r="L4" s="0" t="n">
-        <v>53</v>
-      </c>
-      <c r="M4" s="0" t="n">
-        <v>53</v>
-      </c>
-      <c r="N4" s="0" t="s">
-        <v>193</v>
-      </c>
-      <c r="O4" s="0" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1543,45 +1477,33 @@
         <v>7</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="F5" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="G5" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="G5" s="0" t="s">
-        <v>197</v>
-      </c>
       <c r="H5" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="I5" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="J5" s="0" t="s">
-        <v>193</v>
+      <c r="I5" s="0" t="n">
+        <v>443</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>443</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>193</v>
-      </c>
-      <c r="L5" s="0" t="n">
-        <v>443</v>
-      </c>
-      <c r="M5" s="0" t="n">
-        <v>443</v>
-      </c>
-      <c r="N5" s="0" t="s">
-        <v>193</v>
-      </c>
-      <c r="O5" s="0" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1604,12 +1526,12 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="D10 B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="9.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="9.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="8.52"/>
@@ -1624,7 +1546,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>125</v>
@@ -1633,19 +1555,19 @@
         <v>24</v>
       </c>
       <c r="E1" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="I1" s="0" t="s">
         <v>203</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>204</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>205</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>206</v>
-      </c>
-      <c r="I1" s="0" t="s">
-        <v>207</v>
       </c>
       <c r="J1" s="0" t="s">
         <v>6</v>
@@ -1656,28 +1578,28 @@
         <v>7</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>0</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="J2" s="0" t="s">
         <v>13</v>
@@ -1688,28 +1610,28 @@
         <v>7</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>0</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="F3" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="H3" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="G3" s="0" t="s">
-        <v>194</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>214</v>
-      </c>
       <c r="I3" s="0" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="J3" s="0" t="s">
         <v>13</v>
@@ -1720,28 +1642,28 @@
         <v>7</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="J4" s="0" t="s">
         <v>13</v>
@@ -1765,13 +1687,13 @@
   </sheetPr>
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.05"/>
@@ -1793,10 +1715,10 @@
         <v>37</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="G1" s="0" t="s">
         <v>6</v>
@@ -1810,16 +1732,16 @@
         <v>40</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>217</v>
+        <v>44</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>42</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="G2" s="0" t="s">
         <v>13</v>
@@ -1833,16 +1755,16 @@
         <v>40</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>217</v>
+        <v>44</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>42</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="G3" s="0" t="s">
         <v>13</v>
@@ -1856,16 +1778,16 @@
         <v>40</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>217</v>
+        <v>44</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>45</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="G4" s="0" t="s">
         <v>13</v>
@@ -1879,16 +1801,16 @@
         <v>40</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>217</v>
+        <v>44</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>45</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="G5" s="0" t="s">
         <v>13</v>
@@ -1902,16 +1824,16 @@
         <v>40</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>217</v>
+        <v>44</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>47</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="G6" s="0" t="s">
         <v>13</v>
@@ -1925,16 +1847,16 @@
         <v>40</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>217</v>
+        <v>44</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>47</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="G7" s="0" t="s">
         <v>13</v>
@@ -1954,10 +1876,10 @@
         <v>160</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="G8" s="0" t="s">
         <v>13</v>
@@ -1977,10 +1899,10 @@
         <v>160</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="G9" s="0" t="s">
         <v>13</v>
@@ -2000,10 +1922,10 @@
         <v>163</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="G10" s="0" t="s">
         <v>13</v>
@@ -2023,10 +1945,10 @@
         <v>163</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="G11" s="0" t="s">
         <v>13</v>
@@ -2046,10 +1968,10 @@
         <v>165</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="G12" s="0" t="s">
         <v>13</v>
@@ -2069,10 +1991,10 @@
         <v>165</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="G13" s="0" t="s">
         <v>13</v>
@@ -2097,10 +2019,10 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G22" activeCellId="1" sqref="D10 G22"/>
+      <selection pane="topLeft" activeCell="G22" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.91"/>
@@ -2274,10 +2196,10 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="1" sqref="D10 E4"/>
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.1"/>
@@ -2412,10 +2334,10 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D10 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.88"/>
@@ -2650,10 +2572,10 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D10 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.54"/>
@@ -2781,10 +2703,10 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D10 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.02"/>
@@ -3077,10 +2999,10 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D10 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.38"/>
@@ -3149,10 +3071,10 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D10 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.38"/>
@@ -3320,10 +3242,10 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D10 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.42"/>

</xml_diff>

<commit_message>
Added access policies for interfaces
</commit_message>
<xml_diff>
--- a/all-aci-config.xlsx
+++ b/all-aci-config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="12"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="tenant-tn-vrf" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,6 +23,8 @@
     <sheet name="tenant-filter" sheetId="13" state="visible" r:id="rId14"/>
     <sheet name="tenant-contract" sheetId="14" state="visible" r:id="rId15"/>
     <sheet name="tenant-epg-contract" sheetId="15" state="visible" r:id="rId16"/>
+    <sheet name="fabric-ap-int-policy" sheetId="16" state="visible" r:id="rId17"/>
+    <sheet name="fabric-ap-int-block" sheetId="17" state="visible" r:id="rId18"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="241">
   <si>
     <t xml:space="preserve">tenant</t>
   </si>
@@ -679,6 +681,84 @@
   </si>
   <si>
     <t xml:space="preserve">consumer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">intpolicy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">linktype</t>
+  </si>
+  <si>
+    <t xml:space="preserve">speedpolicy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cdppolicy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lldppolicy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pcpolicy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Firewall-policy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Speed_1G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">default</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LB-policy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c7000-policy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">node</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lacp_active</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chassis-policy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">link</t>
+  </si>
+  <si>
+    <t xml:space="preserve">intname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">intfrom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">intto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eth1_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eth1_10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eth1_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eth1_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eth1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eth1_22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eth1_9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eth1_8</t>
   </si>
 </sst>
 </file>
@@ -786,7 +866,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.02"/>
@@ -911,7 +991,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.44"/>
@@ -1043,7 +1123,7 @@
       <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.24"/>
@@ -1194,7 +1274,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.24"/>
@@ -1315,13 +1395,13 @@
   </sheetPr>
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="9.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="9.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.07"/>
@@ -1529,7 +1609,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="9.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.96"/>
@@ -1691,7 +1771,7 @@
       <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.05"/>
@@ -1997,6 +2077,356 @@
         <v>214</v>
       </c>
       <c r="G13" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="1:1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="7.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="7.54"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>215</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>216</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>220</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>222</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>224</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>222</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>222</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>228</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>229</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>222</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="5.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="7.54"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>231</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>232</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>215</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>233</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>234</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>235</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>224</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>236</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>224</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>238</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>239</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>228</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>240</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>228</v>
+      </c>
+      <c r="F9" s="0" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2022,7 +2452,7 @@
       <selection pane="topLeft" activeCell="G22" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.91"/>
@@ -2199,7 +2629,7 @@
       <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.1"/>
@@ -2337,7 +2767,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.88"/>
@@ -2575,7 +3005,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.54"/>
@@ -2706,7 +3136,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.02"/>
@@ -3002,7 +3432,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.38"/>
@@ -3074,7 +3504,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.38"/>
@@ -3245,7 +3675,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.42"/>

</xml_diff>

<commit_message>
Final testing of switch interface policy assignment playbook
</commit_message>
<xml_diff>
--- a/all-aci-config.xlsx
+++ b/all-aci-config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="16"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="tenant-tn-vrf" sheetId="1" state="visible" r:id="rId2"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="242">
   <si>
     <t xml:space="preserve">tenant</t>
   </si>
@@ -687,6 +687,9 @@
   </si>
   <si>
     <t xml:space="preserve">linktype</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aep</t>
   </si>
   <si>
     <t xml:space="preserve">speedpolicy</t>
@@ -863,10 +866,10 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C3:C5 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.02"/>
@@ -988,10 +991,10 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C3:C5 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.44"/>
@@ -1120,10 +1123,10 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="1" sqref="C3:C5 E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.24"/>
@@ -1271,10 +1274,10 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="C3:C5 B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.24"/>
@@ -1396,10 +1399,10 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="C3:C5 B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="9.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.96"/>
@@ -1606,10 +1609,10 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="C3:C5 B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="9.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.96"/>
@@ -1768,10 +1771,10 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="1" sqref="C3:C5 C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.05"/>
@@ -2096,17 +2099,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="1:1048576"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="7.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="7.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="7.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2129,92 +2132,107 @@
         <v>220</v>
       </c>
       <c r="G1" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="H1" s="0" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>57</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>222</v>
+        <v>151</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>223</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>223</v>
-      </c>
-      <c r="G2" s="0" t="s">
+        <v>224</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>224</v>
+      </c>
+      <c r="H2" s="0" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>57</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>222</v>
+        <v>151</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>223</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>223</v>
-      </c>
-      <c r="G3" s="0" t="s">
+        <v>224</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>224</v>
+      </c>
+      <c r="H3" s="0" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>222</v>
+        <v>151</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>223</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="G4" s="0" t="s">
+        <v>228</v>
+      </c>
+      <c r="H4" s="0" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>222</v>
+        <v>151</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>223</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="G5" s="0" t="s">
+        <v>224</v>
+      </c>
+      <c r="H5" s="0" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2236,11 +2254,11 @@
   </sheetPr>
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C3:C5 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.95"/>
@@ -2255,13 +2273,13 @@
         <v>95</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="E1" s="0" t="s">
         <v>215</v>
@@ -2275,7 +2293,7 @@
         <v>100</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>1</v>
@@ -2284,7 +2302,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>13</v>
@@ -2295,7 +2313,7 @@
         <v>105</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>10</v>
@@ -2304,7 +2322,7 @@
         <v>10</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>13</v>
@@ -2315,7 +2333,7 @@
         <v>110</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>3</v>
@@ -2324,7 +2342,7 @@
         <v>3</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>13</v>
@@ -2335,7 +2353,7 @@
         <v>115</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>5</v>
@@ -2344,7 +2362,7 @@
         <v>5</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="F5" s="0" t="s">
         <v>13</v>
@@ -2355,7 +2373,7 @@
         <v>118</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>2</v>
@@ -2364,7 +2382,7 @@
         <v>2</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F6" s="0" t="s">
         <v>13</v>
@@ -2375,7 +2393,7 @@
         <v>118</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>22</v>
@@ -2384,7 +2402,7 @@
         <v>22</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F7" s="0" t="s">
         <v>13</v>
@@ -2395,7 +2413,7 @@
         <v>121</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>9</v>
@@ -2404,7 +2422,7 @@
         <v>9</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>13</v>
@@ -2415,7 +2433,7 @@
         <v>121</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>8</v>
@@ -2424,7 +2442,7 @@
         <v>8</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="F9" s="0" t="s">
         <v>13</v>
@@ -2449,10 +2467,10 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G22" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="G22" activeCellId="1" sqref="C3:C5 G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.91"/>
@@ -2626,10 +2644,10 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="E4" activeCellId="1" sqref="C3:C5 E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.1"/>
@@ -2764,10 +2782,10 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C3:C5 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.88"/>
@@ -3002,10 +3020,10 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C3:C5 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.54"/>
@@ -3133,10 +3151,10 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C3:C5 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.02"/>
@@ -3429,10 +3447,10 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C3:C5 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.38"/>
@@ -3501,10 +3519,10 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C3:C5 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.38"/>
@@ -3672,10 +3690,10 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C3:C5 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.42"/>

</xml_diff>